<commit_message>
update 15 juni 2024
</commit_message>
<xml_diff>
--- a/TA/Book1.xlsx
+++ b/TA/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jamil\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255546A7-F780-474F-8199-5C0611436F2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CE6B9A-5D15-4E5B-A1FB-8D74FF4E5656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2371494-0D6F-4D29-8E65-A0FC749F8736}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>NIM</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>Rancang Bangun Sistem Kontrol Penyemprotan Cairan Pestisida Otomatis Menggunakan Drone UAV Hexacopter</t>
+  </si>
+  <si>
+    <t>Wisuda</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -457,25 +460,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -485,11 +479,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04A28E4-E0E4-46B4-B4AA-22960535DFC8}">
   <dimension ref="D1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,13 +829,15 @@
       <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="3" spans="4:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D3" s="5">
@@ -850,169 +849,185 @@
       <c r="F3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="17">
+        <v>45352</v>
+      </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>19065002</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="14"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D5" s="4">
+      <c r="D5" s="15">
         <v>19065003</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="14"/>
+      <c r="I5" s="16">
+        <v>45352</v>
+      </c>
     </row>
     <row r="6" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D6" s="19">
+      <c r="D6" s="15">
         <v>19065004</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="15" t="s">
         <v>71</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="14"/>
+      <c r="I6" s="16">
+        <v>45170</v>
+      </c>
     </row>
     <row r="7" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D7" s="4">
+      <c r="D7" s="15">
         <v>19065005</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="14"/>
+      <c r="I7" s="16">
+        <v>45261</v>
+      </c>
     </row>
     <row r="8" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D8" s="19">
+      <c r="D8" s="15">
         <v>19065006</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="14"/>
+      <c r="I8" s="16">
+        <v>45170</v>
+      </c>
     </row>
     <row r="9" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D9" s="19">
+      <c r="D9" s="15">
         <v>19065007</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="15" t="s">
         <v>79</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="14"/>
+      <c r="I9" s="16">
+        <v>45170</v>
+      </c>
     </row>
     <row r="10" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D10" s="4">
+      <c r="D10" s="15">
         <v>19065008</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D11" s="19">
+      <c r="D11" s="15">
         <v>19065009</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="15" t="s">
         <v>83</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="16">
+        <v>45170</v>
+      </c>
     </row>
     <row r="12" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D12" s="4">
+      <c r="D12" s="15">
         <v>19065010</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="15" t="s">
         <v>49</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="14"/>
+      <c r="I12" s="16">
+        <v>45352</v>
+      </c>
     </row>
     <row r="13" spans="4:11" ht="60" x14ac:dyDescent="0.25">
       <c r="D13" s="4">
@@ -1024,13 +1039,15 @@
       <c r="F13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="14"/>
+      <c r="I13" s="16">
+        <v>45352</v>
+      </c>
     </row>
     <row r="14" spans="4:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D14" s="4">
@@ -1042,13 +1059,15 @@
       <c r="F14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="14"/>
+      <c r="I14" s="16">
+        <v>45261</v>
+      </c>
     </row>
     <row r="15" spans="4:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D15" s="4">
@@ -1060,13 +1079,15 @@
       <c r="F15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="14"/>
+      <c r="I15" s="16">
+        <v>45261</v>
+      </c>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
@@ -1077,9 +1098,9 @@
         <v>86</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="14"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D17" s="4">
@@ -1091,13 +1112,15 @@
       <c r="F17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="14"/>
+      <c r="I17" s="16">
+        <v>45261</v>
+      </c>
     </row>
     <row r="18" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D18" s="4">
@@ -1109,13 +1132,15 @@
       <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="14"/>
+      <c r="I18" s="16">
+        <v>45352</v>
+      </c>
     </row>
     <row r="19" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D19" s="4">
@@ -1127,23 +1152,25 @@
       <c r="F19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="14"/>
+      <c r="I19" s="16">
+        <v>45444</v>
+      </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>19065018</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="14"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="8"/>
     </row>
     <row r="21" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D21" s="4">
@@ -1155,13 +1182,15 @@
       <c r="F21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="14"/>
+      <c r="I21" s="16">
+        <v>45444</v>
+      </c>
     </row>
     <row r="22" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D22" s="4">
@@ -1173,13 +1202,15 @@
       <c r="F22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="14"/>
+      <c r="I22" s="16">
+        <v>45261</v>
+      </c>
     </row>
     <row r="23" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D23" s="4">
@@ -1191,13 +1222,15 @@
       <c r="F23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="14"/>
+      <c r="I23" s="16">
+        <v>45261</v>
+      </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D24" s="4">
@@ -1207,9 +1240,9 @@
         <v>89</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="14"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D25" s="4">
@@ -1221,13 +1254,15 @@
       <c r="F25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="14"/>
+      <c r="I25" s="16">
+        <v>45261</v>
+      </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D26" s="4">
@@ -1237,37 +1272,39 @@
         <v>90</v>
       </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="14"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="15">
+      <c r="D27" s="12">
         <v>19065025</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="14"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D28" s="19">
+      <c r="D28" s="15">
         <v>19065026</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="15" t="s">
         <v>74</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="14"/>
+      <c r="I28" s="16">
+        <v>45170</v>
+      </c>
     </row>
     <row r="29" spans="4:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D29" s="4">
@@ -1279,13 +1316,15 @@
       <c r="F29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I29" s="14"/>
+      <c r="I29" s="16">
+        <v>45261</v>
+      </c>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D30" s="4">
@@ -1295,9 +1334,9 @@
         <v>88</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="14"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="8"/>
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D31" s="4">
@@ -1307,45 +1346,49 @@
         <v>87</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="14"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="8"/>
     </row>
     <row r="32" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D32" s="19">
+      <c r="D32" s="15">
         <v>19065030</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="15" t="s">
         <v>76</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="I32" s="14"/>
+      <c r="I32" s="16">
+        <v>45170</v>
+      </c>
     </row>
     <row r="33" spans="4:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="D33" s="19">
+      <c r="D33" s="15">
         <v>19065031</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="15" t="s">
         <v>66</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G33" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="14"/>
+      <c r="I33" s="16">
+        <v>45170</v>
+      </c>
     </row>
     <row r="34" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D34" s="4">
@@ -1357,13 +1400,15 @@
       <c r="F34" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="H34" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="14"/>
+      <c r="I34" s="16">
+        <v>45352</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 27 mai 2025
</commit_message>
<xml_diff>
--- a/TA/Book1.xlsx
+++ b/TA/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jamil\TA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jamil\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CE6B9A-5D15-4E5B-A1FB-8D74FF4E5656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C8D4EF-4243-42CB-B947-FFFC60A77FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2371494-0D6F-4D29-8E65-A0FC749F8736}"/>
   </bookViews>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>NIM</t>
   </si>
@@ -312,6 +307,18 @@
   </si>
   <si>
     <t>Wisuda</t>
+  </si>
+  <si>
+    <t>HUBUNGAN KESIAPAN GURU DAN SARANA PEMBELAJARAN TERHADAP IMPLEMENTASI KURIKULUM MARDEKA DI JURUSAN TEKNIK ELEKTRONIKA PADA SMK NEGERI 5 PADANG</t>
+  </si>
+  <si>
+    <t>Dr. Dedy Irfan, S.Pd., M.Kom / 5327, Ilmiyati Rahmy Jasril, S.Pd., M.Pd.T / 5340</t>
+  </si>
+  <si>
+    <t>Prototipe mesin pemotong rumput berbasis arduino uno dengan pengendali android</t>
+  </si>
+  <si>
+    <t>Sartika Anori, S.Pd.,M.Pd.T / 182038, Winda Agustiarmi, S.Pd.,M.Pd.T / 192042</t>
   </si>
 </sst>
 </file>
@@ -439,16 +446,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -457,9 +460,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -475,7 +475,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -487,6 +486,24 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,15 +821,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04A28E4-E0E4-46B4-B4AA-22960535DFC8}">
   <dimension ref="D1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="67.85546875" customWidth="1"/>
+    <col min="6" max="6" width="67.85546875" style="15" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="34.140625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -820,593 +837,609 @@
   <sheetData>
     <row r="1" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>19065001</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="13">
         <v>45352</v>
       </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>19065002</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="8"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>19065003</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="12">
         <v>45352</v>
       </c>
     </row>
     <row r="6" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D6" s="15">
+      <c r="D6" s="11">
         <v>19065004</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="12">
         <v>45170</v>
       </c>
     </row>
     <row r="7" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <v>19065005</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="12">
         <v>45261</v>
       </c>
     </row>
     <row r="8" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <v>19065006</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="12">
         <v>45170</v>
       </c>
     </row>
     <row r="9" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D9" s="15">
+      <c r="D9" s="11">
         <v>19065007</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="12">
         <v>45170</v>
       </c>
     </row>
     <row r="10" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D10" s="15">
+      <c r="D10" s="11">
         <v>19065008</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="12">
+        <v>45627</v>
+      </c>
     </row>
     <row r="11" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <v>19065009</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="12">
         <v>45170</v>
       </c>
     </row>
     <row r="12" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <v>19065010</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="12">
         <v>45352</v>
       </c>
     </row>
     <row r="13" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>19065011</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="12">
         <v>45352</v>
       </c>
     </row>
     <row r="14" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>19065012</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="12">
         <v>45261</v>
       </c>
     </row>
     <row r="15" spans="4:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="D15" s="4">
+      <c r="D15" s="2">
         <v>19065013</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="12">
         <v>45261</v>
       </c>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="4">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
         <v>19065014</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="8"/>
+      <c r="F16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="12">
+        <v>45717</v>
+      </c>
     </row>
     <row r="17" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <v>19065015</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="12">
         <v>45261</v>
       </c>
     </row>
     <row r="18" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D18" s="4">
+      <c r="D18" s="2">
         <v>19065016</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="12">
         <v>45352</v>
       </c>
     </row>
     <row r="19" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <v>19065017</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="12">
         <v>45444</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="12">
+      <c r="D20" s="9">
         <v>19065018</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D21" s="4">
+      <c r="D21" s="2">
         <v>19065019</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="12">
         <v>45444</v>
       </c>
     </row>
     <row r="22" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D22" s="4">
+      <c r="D22" s="2">
         <v>19065020</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="12">
         <v>45261</v>
       </c>
     </row>
     <row r="23" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D23" s="4">
+      <c r="D23" s="2">
         <v>19065021</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="16">
+      <c r="I23" s="12">
         <v>45261</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="4">
+      <c r="D24" s="9">
         <v>19065022</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="8"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D25" s="4">
+      <c r="D25" s="2">
         <v>19065023</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="12">
         <v>45261</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="4">
+      <c r="D26" s="2">
         <v>19065024</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="8"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="5"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="12">
+      <c r="D27" s="9">
         <v>19065025</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="14"/>
     </row>
     <row r="28" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D28" s="15">
+      <c r="D28" s="11">
         <v>19065026</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="16">
+      <c r="I28" s="12">
         <v>45170</v>
       </c>
     </row>
     <row r="29" spans="4:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="D29" s="4">
+      <c r="D29" s="2">
         <v>19065027</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="I29" s="16">
+      <c r="I29" s="12">
         <v>45261</v>
       </c>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="4">
+    <row r="30" spans="4:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
         <v>19065028</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="8"/>
+      <c r="F30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="4">
+      <c r="D31" s="2">
         <v>19065029</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="8"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D32" s="15">
+      <c r="D32" s="11">
         <v>19065030</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="I32" s="16">
+      <c r="I32" s="12">
         <v>45170</v>
       </c>
     </row>
     <row r="33" spans="4:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="D33" s="15">
+      <c r="D33" s="11">
         <v>19065031</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="16">
+      <c r="I33" s="12">
         <v>45170</v>
       </c>
     </row>
     <row r="34" spans="4:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D34" s="4">
+      <c r="D34" s="2">
         <v>19065032</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H34" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="16">
+      <c r="I34" s="12">
         <v>45352</v>
       </c>
     </row>

</xml_diff>